<commit_message>
support for method variants implemented
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/ASTA_Index_Current.xlsx
+++ b/src/sastadev/data/methods/ASTA_Index_Current.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1C8F41-9D63-4B22-BAD9-46C68C037D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A1AA0F-057A-4F74-9225-A2AFF8E7EDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -602,9 +602,6 @@
     <t>unused2</t>
   </si>
   <si>
-    <t>asta_2019</t>
-  </si>
-  <si>
     <t>asta_future</t>
   </si>
   <si>
@@ -633,6 +630,9 @@
   </si>
   <si>
     <t>noun en verb lemmas split up; deze moet verdwijnen</t>
+  </si>
+  <si>
+    <t>astae</t>
   </si>
 </sst>
 </file>
@@ -1015,10 +1015,10 @@
   <dimension ref="A1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomRight" activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,7 +1073,7 @@
         <v>129</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>183</v>
@@ -1125,7 +1125,7 @@
         <v>130</v>
       </c>
       <c r="R2" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="U2" t="s">
         <v>136</v>
@@ -1243,7 +1243,7 @@
         <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E7" t="s">
         <v>104</v>
@@ -1339,7 +1339,7 @@
         <v>130</v>
       </c>
       <c r="U10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
@@ -1474,7 +1474,7 @@
         <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E16" t="s">
         <v>110</v>
@@ -1497,7 +1497,7 @@
         <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E17" t="s">
         <v>108</v>
@@ -1520,7 +1520,7 @@
         <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E18" t="s">
         <v>106</v>
@@ -1839,7 +1839,7 @@
         <v>80</v>
       </c>
       <c r="D30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>89</v>
@@ -1911,7 +1911,7 @@
         <v>83</v>
       </c>
       <c r="D33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>92</v>
@@ -1937,7 +1937,7 @@
         <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>93</v>
@@ -1963,7 +1963,7 @@
         <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>94</v>
@@ -1986,7 +1986,7 @@
         <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>95</v>
@@ -2009,7 +2009,7 @@
         <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>96</v>
@@ -2032,7 +2032,7 @@
         <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>98</v>
@@ -2084,7 +2084,7 @@
         <v>103</v>
       </c>
       <c r="D40" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>123</v>
@@ -2130,7 +2130,7 @@
         <v>128</v>
       </c>
       <c r="D42" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>127</v>
@@ -2197,7 +2197,7 @@
         <v>149</v>
       </c>
       <c r="U44" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
@@ -2243,7 +2243,7 @@
         <v>130</v>
       </c>
       <c r="R46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="U46" t="s">
         <v>158</v>
@@ -2272,7 +2272,7 @@
         <v>149</v>
       </c>
       <c r="U47" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
@@ -2303,7 +2303,7 @@
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D49" t="s">
         <v>148</v>
@@ -2315,7 +2315,7 @@
         <v>15</v>
       </c>
       <c r="K49" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L49" t="s">
         <v>15</v>
@@ -2324,13 +2324,13 @@
         <v>130</v>
       </c>
       <c r="O49" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q49" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U49" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update ASTA K, M and XXX
</commit_message>
<xml_diff>
--- a/src/sastadev/data/methods/ASTA_Index_Current.xlsx
+++ b/src/sastadev/data/methods/ASTA_Index_Current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\jodijk\myprograms\python\sastacode\mysastadev\src\sastadev\data\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31618B29-DAA8-4A9A-A13C-3315898B058B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACDC261-39AA-43BF-A77B-999A06D62FD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,9 +452,6 @@
     <t>//node[%ASTA_kopww%]</t>
   </si>
   <si>
-    <t>//node[@pt="ww" and %ASTA_modalww%]</t>
-  </si>
-  <si>
     <t>SEM PAR, sp</t>
   </si>
   <si>
@@ -639,6 +636,9 @@
   </si>
   <si>
     <t>SSZX</t>
+  </si>
+  <si>
+    <t>//node[@pt="ww" and %ASTA_modalww% and not(%ASTA_XXX%)]</t>
   </si>
 </sst>
 </file>
@@ -1018,13 +1018,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W49"/>
+  <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomRight" activeCell="A50" sqref="A50:V50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1079,22 +1079,22 @@
         <v>129</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>11</v>
@@ -1122,7 +1122,7 @@
         <v>135</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L2" t="s">
         <v>15</v>
@@ -1131,7 +1131,7 @@
         <v>130</v>
       </c>
       <c r="R2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="U2" t="s">
         <v>136</v>
@@ -1180,7 +1180,7 @@
         <v>12</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L4" t="s">
         <v>15</v>
@@ -1200,7 +1200,7 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F5" t="s">
         <v>100</v>
@@ -1226,7 +1226,7 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F6" t="s">
         <v>101</v>
@@ -1249,7 +1249,7 @@
         <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E7" t="s">
         <v>104</v>
@@ -1304,13 +1304,13 @@
         <v>25</v>
       </c>
       <c r="F9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
       <c r="K9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L9" t="s">
         <v>15</v>
@@ -1336,7 +1336,7 @@
         <v>15</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L10" t="s">
         <v>15</v>
@@ -1345,7 +1345,7 @@
         <v>130</v>
       </c>
       <c r="U10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">
@@ -1428,7 +1428,7 @@
         <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H14" t="s">
         <v>15</v>
@@ -1446,7 +1446,7 @@
         <v>130</v>
       </c>
       <c r="Q14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="U14" t="s">
         <v>38</v>
@@ -1480,13 +1480,13 @@
         <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E16" t="s">
         <v>110</v>
       </c>
       <c r="F16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H16" t="s">
         <v>15</v>
@@ -1503,13 +1503,13 @@
         <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" t="s">
         <v>108</v>
       </c>
       <c r="F17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H17" t="s">
         <v>15</v>
@@ -1526,7 +1526,7 @@
         <v>56</v>
       </c>
       <c r="D18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E18" t="s">
         <v>106</v>
@@ -1564,7 +1564,7 @@
         <v>9</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>15</v>
@@ -1574,7 +1574,7 @@
         <v>130</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
@@ -1597,7 +1597,7 @@
         <v>15</v>
       </c>
       <c r="K20" t="s">
-        <v>138</v>
+        <v>200</v>
       </c>
       <c r="L20" t="s">
         <v>15</v>
@@ -1606,7 +1606,7 @@
         <v>130</v>
       </c>
       <c r="Q20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
@@ -1626,7 +1626,7 @@
         <v>8</v>
       </c>
       <c r="K21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L21" t="s">
         <v>15</v>
@@ -1635,7 +1635,7 @@
         <v>130</v>
       </c>
       <c r="Q21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="U21" t="s">
         <v>132</v>
@@ -1661,7 +1661,7 @@
         <v>10</v>
       </c>
       <c r="K22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L22" t="s">
         <v>15</v>
@@ -1670,7 +1670,7 @@
         <v>130</v>
       </c>
       <c r="Q22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -1713,13 +1713,13 @@
         <v>37</v>
       </c>
       <c r="L24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N24" t="s">
         <v>130</v>
       </c>
       <c r="U24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
@@ -1733,13 +1733,13 @@
         <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H25" t="s">
         <v>15</v>
       </c>
       <c r="K25" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L25" t="s">
         <v>15</v>
@@ -1762,13 +1762,13 @@
         <v>37</v>
       </c>
       <c r="L26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N26" t="s">
         <v>130</v>
       </c>
       <c r="U26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
@@ -1802,7 +1802,7 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F28" t="s">
         <v>28</v>
@@ -1817,7 +1817,7 @@
         <v>15</v>
       </c>
       <c r="N28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.3">
@@ -1848,7 +1848,7 @@
         <v>80</v>
       </c>
       <c r="D30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>89</v>
@@ -1900,7 +1900,7 @@
         <v>91</v>
       </c>
       <c r="F32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H32" t="s">
         <v>15</v>
@@ -1920,13 +1920,13 @@
         <v>83</v>
       </c>
       <c r="D33" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H33" t="s">
         <v>15</v>
@@ -1946,13 +1946,13 @@
         <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H34" t="s">
         <v>15</v>
@@ -1972,7 +1972,7 @@
         <v>85</v>
       </c>
       <c r="D35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>94</v>
@@ -1995,7 +1995,7 @@
         <v>86</v>
       </c>
       <c r="D36" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>95</v>
@@ -2018,7 +2018,7 @@
         <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>96</v>
@@ -2041,13 +2041,13 @@
         <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>98</v>
       </c>
       <c r="F38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H38" t="s">
         <v>15</v>
@@ -2073,7 +2073,7 @@
         <v>119</v>
       </c>
       <c r="F39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H39" t="s">
         <v>120</v>
@@ -2093,7 +2093,7 @@
         <v>103</v>
       </c>
       <c r="D40" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E40" s="4" t="s">
         <v>123</v>
@@ -2139,13 +2139,13 @@
         <v>128</v>
       </c>
       <c r="D42" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>127</v>
       </c>
       <c r="F42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H42" t="s">
         <v>120</v>
@@ -2168,7 +2168,7 @@
         <v>16</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F43" t="s">
         <v>28</v>
@@ -2183,67 +2183,67 @@
         <v>15</v>
       </c>
       <c r="N43" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>146</v>
+      </c>
+      <c r="D44" t="s">
         <v>147</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H44" t="s">
+        <v>15</v>
+      </c>
+      <c r="K44" t="s">
+        <v>169</v>
+      </c>
+      <c r="L44" t="s">
+        <v>15</v>
+      </c>
+      <c r="N44" t="s">
         <v>148</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="H44" t="s">
-        <v>15</v>
-      </c>
-      <c r="K44" t="s">
-        <v>170</v>
-      </c>
-      <c r="L44" t="s">
-        <v>15</v>
-      </c>
-      <c r="N44" t="s">
-        <v>149</v>
-      </c>
       <c r="U44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>149</v>
+      </c>
+      <c r="D45" t="s">
         <v>150</v>
       </c>
-      <c r="D45" t="s">
+      <c r="H45" t="s">
+        <v>15</v>
+      </c>
+      <c r="K45" t="s">
         <v>151</v>
-      </c>
-      <c r="H45" t="s">
-        <v>15</v>
-      </c>
-      <c r="K45" t="s">
-        <v>152</v>
       </c>
       <c r="L45" t="s">
         <v>120</v>
       </c>
       <c r="N45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D46" t="s">
         <v>18</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H46" t="s">
         <v>120</v>
@@ -2255,50 +2255,50 @@
         <v>130</v>
       </c>
       <c r="R46" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E47" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H47" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47" t="s">
         <v>172</v>
-      </c>
-      <c r="H47" t="s">
-        <v>15</v>
-      </c>
-      <c r="K47" t="s">
-        <v>173</v>
       </c>
       <c r="L47" t="s">
         <v>120</v>
       </c>
       <c r="N47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="U47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D48" t="s">
         <v>18</v>
       </c>
       <c r="E48" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F48" t="s">
         <v>176</v>
-      </c>
-      <c r="F48" t="s">
-        <v>177</v>
       </c>
       <c r="H48" t="s">
         <v>120</v>
@@ -2310,40 +2310,43 @@
         <v>130</v>
       </c>
       <c r="U48" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" t="s">
+        <v>147</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H49" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49" t="s">
+        <v>191</v>
+      </c>
+      <c r="L49" t="s">
+        <v>15</v>
+      </c>
+      <c r="N49" t="s">
+        <v>130</v>
+      </c>
+      <c r="O49" t="s">
+        <v>193</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>190</v>
+      </c>
+      <c r="U49" t="s">
         <v>189</v>
       </c>
-      <c r="D49" t="s">
-        <v>148</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="H49" t="s">
-        <v>15</v>
-      </c>
-      <c r="K49" t="s">
-        <v>192</v>
-      </c>
-      <c r="L49" t="s">
-        <v>15</v>
-      </c>
-      <c r="N49" t="s">
-        <v>130</v>
-      </c>
-      <c r="O49" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>191</v>
-      </c>
-      <c r="U49" t="s">
-        <v>190</v>
-      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="E50" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:W49" xr:uid="{356449EB-3FBE-4443-8528-03CDC854A576}"/>

</xml_diff>